<commit_message>
update model_Sim with AV2016lag data
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_PlanInfo_AV2016.xlsx
+++ b/Inputs_data/NYCTRS_PlanInfo_AV2016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE51196-CE53-4A83-8837-C1F495B5697C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9FE95-2060-4F91-B249-D035AB3106F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="44" r:id="rId1"/>
@@ -1391,8 +1391,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1406,7 @@
     <col min="7" max="7" width="20.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="11" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="14.85546875" customWidth="1"/>
     <col min="12" max="13" width="17.5703125" customWidth="1"/>
     <col min="14" max="15" width="27.28515625" customWidth="1"/>
@@ -1511,19 +1511,19 @@
         <v>2010</v>
       </c>
       <c r="F8" s="65">
-        <v>20524023</v>
+        <v>20524023000</v>
       </c>
       <c r="G8" s="66">
         <v>22</v>
       </c>
       <c r="H8" s="65">
-        <v>21099902</v>
+        <v>21099902000</v>
       </c>
       <c r="I8" s="66">
         <v>16</v>
       </c>
       <c r="J8" s="67">
-        <v>1841243</v>
+        <v>1841243000</v>
       </c>
       <c r="K8" s="68" t="s">
         <v>47</v>
@@ -1544,19 +1544,19 @@
         <v>2011</v>
       </c>
       <c r="F9" s="71">
-        <v>1329890</v>
+        <v>1329890000</v>
       </c>
       <c r="G9" s="66">
         <v>15</v>
       </c>
       <c r="H9" s="71">
-        <v>1142813</v>
+        <v>1142813000</v>
       </c>
       <c r="I9" s="70">
         <v>10</v>
       </c>
       <c r="J9" s="72">
-        <v>157299</v>
+        <v>157299000</v>
       </c>
       <c r="K9" s="63" t="s">
         <v>35</v>
@@ -1577,19 +1577,19 @@
         <v>2012</v>
       </c>
       <c r="F10" s="71">
-        <v>778617</v>
+        <v>778617000</v>
       </c>
       <c r="G10" s="66">
         <v>15</v>
       </c>
       <c r="H10" s="71">
-        <v>714347</v>
+        <v>714347000</v>
       </c>
       <c r="I10" s="70">
         <v>11</v>
       </c>
       <c r="J10" s="72">
-        <v>92094</v>
+        <v>92094000</v>
       </c>
       <c r="K10" s="63" t="s">
         <v>35</v>
@@ -1610,19 +1610,19 @@
         <v>2013</v>
       </c>
       <c r="F11" s="71">
-        <v>2065938</v>
+        <v>2065938000</v>
       </c>
       <c r="G11" s="66">
         <v>15</v>
       </c>
       <c r="H11" s="71">
-        <v>2007638</v>
+        <v>2007638000</v>
       </c>
       <c r="I11" s="70">
         <v>12</v>
       </c>
       <c r="J11" s="72">
-        <v>244358</v>
+        <v>244358000</v>
       </c>
       <c r="K11" s="63" t="s">
         <v>35</v>
@@ -1643,19 +1643,19 @@
         <v>2014</v>
       </c>
       <c r="F12" s="71">
-        <v>992710</v>
+        <v>992710000</v>
       </c>
       <c r="G12" s="66">
         <v>15</v>
       </c>
       <c r="H12" s="71">
-        <v>1015096</v>
+        <v>1015096000</v>
       </c>
       <c r="I12" s="70">
         <v>13</v>
       </c>
       <c r="J12" s="72">
-        <v>117417</v>
+        <v>117417000</v>
       </c>
       <c r="K12" s="63" t="s">
         <v>35</v>
@@ -1676,19 +1676,19 @@
         <v>2014</v>
       </c>
       <c r="F13" s="71">
-        <v>2239586</v>
+        <v>2239586000</v>
       </c>
       <c r="G13" s="66">
         <v>20</v>
       </c>
       <c r="H13" s="71">
-        <v>2332248</v>
+        <v>2332248000</v>
       </c>
       <c r="I13" s="70">
         <v>18</v>
       </c>
       <c r="J13" s="72">
-        <v>224142</v>
+        <v>224142000</v>
       </c>
       <c r="K13" s="63" t="s">
         <v>35</v>
@@ -1709,19 +1709,19 @@
         <v>2015</v>
       </c>
       <c r="F14" s="71">
-        <v>734444</v>
+        <v>734444000</v>
       </c>
       <c r="G14" s="66">
         <v>15</v>
       </c>
       <c r="H14" s="71">
-        <v>785855</v>
+        <v>785855000</v>
       </c>
       <c r="I14" s="70">
         <v>14</v>
       </c>
       <c r="J14" s="72">
-        <v>86870</v>
+        <v>86870000</v>
       </c>
       <c r="K14" s="63" t="s">
         <v>35</v>
@@ -1742,19 +1742,19 @@
         <v>2016</v>
       </c>
       <c r="F15" s="71">
-        <v>-848432</v>
+        <v>-848432000</v>
       </c>
       <c r="G15" s="66">
         <v>15</v>
       </c>
       <c r="H15" s="71">
-        <v>-848432</v>
+        <v>-848432000</v>
       </c>
       <c r="I15" s="70">
         <v>15</v>
       </c>
       <c r="J15" s="72">
-        <v>-100352</v>
+        <v>-100352000</v>
       </c>
       <c r="K15" s="63" t="s">
         <v>35</v>
@@ -1997,7 +1997,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2515,7 +2515,7 @@
   <dimension ref="A3:L23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update with OYLM for only amort payments
</commit_message>
<xml_diff>
--- a/Inputs_data/NYCTRS_PlanInfo_AV2016.xlsx
+++ b/Inputs_data/NYCTRS_PlanInfo_AV2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9FE95-2060-4F91-B249-D035AB3106F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A80B103-CB04-43C5-917E-AA0501E5BD26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1407,7 +1407,7 @@
     <col min="8" max="8" width="16.28515625" style="11" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
     <col min="12" max="13" width="17.5703125" customWidth="1"/>
     <col min="14" max="15" width="27.28515625" customWidth="1"/>
     <col min="16" max="19" width="14.5703125" customWidth="1"/>

</xml_diff>